<commit_message>
Add tags to it_emx_datatypes.xlsx
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_datatypes.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_datatypes.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="0" windowWidth="33860" windowHeight="18480" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22700" windowHeight="14720" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
     <sheet name="entities" sheetId="3" r:id="rId2"/>
     <sheet name="attributes" sheetId="4" r:id="rId3"/>
-    <sheet name="it_emx_datatypes_TypeTest" sheetId="1" r:id="rId4"/>
-    <sheet name="it_emx_datatypes_TypeTestRef" sheetId="2" r:id="rId5"/>
+    <sheet name="tags" sheetId="6" r:id="rId4"/>
+    <sheet name="it_emx_datatypes_TypeTest" sheetId="1" r:id="rId5"/>
+    <sheet name="it_emx_datatypes_TypeTestRef" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="287">
   <si>
     <t>text</t>
   </si>
@@ -836,6 +837,54 @@
   </si>
   <si>
     <t>MOLGENIS datatypes test package</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>objectIRI</t>
+  </si>
+  <si>
+    <t>relationIRI</t>
+  </si>
+  <si>
+    <t>relationLabel</t>
+  </si>
+  <si>
+    <t>codeSystem</t>
+  </si>
+  <si>
+    <t>dct:title</t>
+  </si>
+  <si>
+    <t>isAssociatedWith</t>
+  </si>
+  <si>
+    <t>http://molgenis.org#isAssociatedWith</t>
+  </si>
+  <si>
+    <t>mlg</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/title</t>
+  </si>
+  <si>
+    <t>dct:identifier</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/identifier</t>
+  </si>
+  <si>
+    <t>dct</t>
+  </si>
+  <si>
+    <t>mlg:TestEntity</t>
+  </si>
+  <si>
+    <t>http://molgenis.org#TestEntity</t>
+  </si>
+  <si>
+    <t>tags</t>
   </si>
 </sst>
 </file>
@@ -891,9 +940,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -948,7 +999,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -995,6 +1046,8 @@
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1355,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1367,9 +1420,10 @@
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1385,8 +1439,11 @@
       <c r="E1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1399,8 +1456,11 @@
       <c r="D2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1414,7 +1474,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1428,7 +1488,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -1455,1583 +1515,1598 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>161</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>258</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>92</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>150</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>138</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>154</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>56</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" t="s">
         <v>261</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
       <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>172</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>261</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="T3" t="s">
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>173</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>59</v>
       </c>
       <c r="B4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" t="s">
         <v>262</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
       <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>262</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>67</v>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>262</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>67</v>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
       <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
         <v>170</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>262</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>146</v>
       </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="T7" t="s">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
         <v>171</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>147</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>262</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
       <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
         <v>145</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>148</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>262</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
       <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>148</v>
       </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
         <v>145</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>174</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>262</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>261</v>
       </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+      <c r="U10" t="s">
         <v>175</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>262</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>68</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>261</v>
       </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
       <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>3</v>
-      </c>
-      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>152</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>262</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>151</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>261</v>
       </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>162</v>
       </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>153</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>262</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>151</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>261</v>
       </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
       <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
         <v>163</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>262</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="4">
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
         <v>41852</v>
       </c>
-      <c r="N14" t="b">
-        <v>1</v>
-      </c>
-      <c r="T14" t="s">
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
         <v>179</v>
       </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>262</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
       <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
         <v>42095</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>180</v>
       </c>
-      <c r="U15" t="s">
+      <c r="V15" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>262</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>6</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>262</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
       <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
         <v>6</v>
       </c>
-      <c r="N17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
         <v>181</v>
       </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>262</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>71</v>
       </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
-      <c r="H18">
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>10.234</v>
       </c>
-      <c r="N18" t="b">
-        <v>1</v>
-      </c>
-      <c r="T18" t="s">
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
         <v>182</v>
       </c>
-      <c r="U18" t="s">
+      <c r="V18" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>262</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
       <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>15.666</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>183</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>262</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>164</v>
       </c>
-      <c r="N20" t="b">
-        <v>1</v>
-      </c>
-      <c r="T20" t="s">
+      <c r="O20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
         <v>184</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>262</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
       <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
         <v>7</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>185</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>262</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
         <v>80</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>8</v>
       </c>
-      <c r="N22" t="b">
-        <v>1</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="O22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>262</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>79</v>
       </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
       <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
         <v>80</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>10</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>187</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>262</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="b">
-        <v>0</v>
-      </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
         <v>11</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>262</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
       <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
         <v>165</v>
       </c>
-      <c r="N25" t="b">
-        <v>1</v>
-      </c>
-      <c r="T25" t="s">
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="s">
         <v>188</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>262</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="E26" t="b">
-        <v>0</v>
-      </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
         <v>166</v>
       </c>
-      <c r="N26" t="b">
-        <v>1</v>
-      </c>
-      <c r="T26" t="s">
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" t="s">
         <v>189</v>
       </c>
-      <c r="U26" t="s">
+      <c r="V26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>262</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="E27" t="b">
-        <v>0</v>
-      </c>
       <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
         <v>167</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>190</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>262</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>66</v>
       </c>
-      <c r="E28" t="b">
-        <v>0</v>
-      </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
-      <c r="H28">
-        <v>3</v>
-      </c>
-      <c r="N28" t="b">
-        <v>1</v>
-      </c>
-      <c r="T28" t="s">
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+      <c r="U28" t="s">
         <v>191</v>
       </c>
-      <c r="U28" t="s">
+      <c r="V28" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>262</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>66</v>
       </c>
-      <c r="E29" t="b">
-        <v>0</v>
-      </c>
       <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="U29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="V29" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>262</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>66</v>
       </c>
-      <c r="E30" t="b">
-        <v>0</v>
-      </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="H30">
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>6</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>10</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>192</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>262</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
       <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <v>77</v>
       </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="T31" t="s">
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="U31" t="s">
         <v>193</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>262</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>75</v>
       </c>
-      <c r="E32" t="b">
-        <v>0</v>
-      </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
-      <c r="H32">
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <v>12342151234</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>194</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>262</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>75</v>
       </c>
-      <c r="E33" t="b">
-        <v>0</v>
-      </c>
       <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>12342151234</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>262</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>75</v>
       </c>
-      <c r="E34" t="b">
-        <v>0</v>
-      </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
-      <c r="H34">
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34">
         <v>5</v>
       </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
       <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
         <v>10</v>
       </c>
-      <c r="N34" t="b">
-        <v>1</v>
-      </c>
-      <c r="T34" t="s">
+      <c r="O34" t="b">
+        <v>1</v>
+      </c>
+      <c r="U34" t="s">
         <v>195</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>262</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
       <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
         <v>10</v>
       </c>
-      <c r="N35" t="b">
-        <v>1</v>
-      </c>
-      <c r="T35" t="s">
+      <c r="O35" t="b">
+        <v>1</v>
+      </c>
+      <c r="U35" t="s">
         <v>196</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>262</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>76</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>261</v>
       </c>
-      <c r="E36" t="b">
-        <v>0</v>
-      </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="N36" t="b">
-        <v>1</v>
-      </c>
-      <c r="T36" t="s">
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
+      <c r="U36" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>262</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>76</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>261</v>
       </c>
-      <c r="E37" t="b">
-        <v>0</v>
-      </c>
       <c r="F37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C38" t="s">
         <v>262</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>65</v>
       </c>
-      <c r="E38" t="b">
-        <v>0</v>
-      </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
-      <c r="H38" t="s">
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
         <v>38</v>
       </c>
-      <c r="N38" t="b">
-        <v>1</v>
-      </c>
-      <c r="T38" t="s">
+      <c r="O38" t="b">
+        <v>1</v>
+      </c>
+      <c r="U38" t="s">
         <v>198</v>
       </c>
-      <c r="U38" t="s">
+      <c r="V38" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>262</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>65</v>
       </c>
-      <c r="E39" t="b">
-        <v>0</v>
-      </c>
       <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
         <v>39</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>199</v>
       </c>
-      <c r="U39" t="s">
+      <c r="V39" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>262</v>
       </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E40" t="b">
+      <c r="D40" t="s">
         <v>0</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
         <v>40</v>
       </c>
-      <c r="U40" t="s">
+      <c r="V40" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>262</v>
       </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" t="b">
+      <c r="D41" t="s">
         <v>0</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
         <v>41</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>200</v>
       </c>
-      <c r="U41" t="s">
+      <c r="V41" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>262</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>77</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>261</v>
       </c>
-      <c r="E42" t="b">
-        <v>0</v>
-      </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="N42" t="b">
-        <v>1</v>
-      </c>
-      <c r="T42" t="s">
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" t="b">
+        <v>1</v>
+      </c>
+      <c r="U42" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>262</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>77</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>261</v>
       </c>
-      <c r="E43" t="b">
-        <v>0</v>
-      </c>
       <c r="F43" t="b">
-        <v>1</v>
-      </c>
-      <c r="T43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="U43" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>93</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>262</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>65</v>
       </c>
-      <c r="E44" t="b">
-        <v>0</v>
-      </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
         <v>38</v>
       </c>
-      <c r="O44" t="b">
-        <v>0</v>
-      </c>
-      <c r="T44" t="s">
+      <c r="P44" t="b">
+        <v>0</v>
+      </c>
+      <c r="U44" t="s">
         <v>203</v>
       </c>
-      <c r="U44" t="s">
+      <c r="V44" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>94</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>262</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>65</v>
       </c>
-      <c r="E45" t="b">
-        <v>0</v>
-      </c>
       <c r="F45" t="b">
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
         <v>168</v>
       </c>
-      <c r="O45" t="b">
-        <v>0</v>
-      </c>
-      <c r="T45" t="s">
+      <c r="P45" t="b">
+        <v>0</v>
+      </c>
+      <c r="U45" t="s">
         <v>204</v>
       </c>
-      <c r="U45" t="s">
+      <c r="V45" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>96</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>262</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>65</v>
       </c>
-      <c r="E46" t="b">
-        <v>0</v>
-      </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
-      <c r="P46" t="b">
-        <v>1</v>
-      </c>
-      <c r="U46" t="s">
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="b">
+        <v>1</v>
+      </c>
+      <c r="V46" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>98</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>262</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" t="b">
-        <v>0</v>
-      </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
-      <c r="P47" t="b">
-        <v>1</v>
-      </c>
-      <c r="T47" t="s">
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="b">
+        <v>1</v>
+      </c>
+      <c r="U47" t="s">
         <v>205</v>
       </c>
-      <c r="U47" t="s">
+      <c r="V47" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>134</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>262</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>77</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>261</v>
       </c>
-      <c r="E48" t="b">
-        <v>0</v>
-      </c>
       <c r="F48" t="b">
-        <v>1</v>
-      </c>
-      <c r="P48" t="b">
-        <v>1</v>
-      </c>
-      <c r="T48" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q48" t="b">
+        <v>1</v>
+      </c>
+      <c r="U48" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>256</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>262</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>257</v>
       </c>
-      <c r="E49" t="b">
-        <v>0</v>
-      </c>
       <c r="F49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>139</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>262</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
       <c r="F50" t="b">
-        <v>1</v>
-      </c>
-      <c r="M50" t="b">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="N50" t="b">
+        <v>1</v>
+      </c>
+      <c r="S50" t="s">
         <v>142</v>
       </c>
-      <c r="T50" t="s">
+      <c r="U50" t="s">
         <v>207</v>
       </c>
-      <c r="U50" t="s">
+      <c r="V50" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>137</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>262</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>66</v>
       </c>
-      <c r="E51" t="b">
-        <v>0</v>
-      </c>
       <c r="F51" t="b">
-        <v>1</v>
-      </c>
-      <c r="M51" t="b">
-        <v>1</v>
-      </c>
-      <c r="R51" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="N51" t="b">
+        <v>1</v>
+      </c>
+      <c r="S51" t="s">
         <v>29</v>
       </c>
-      <c r="T51" t="s">
+      <c r="U51" t="s">
         <v>208</v>
       </c>
-      <c r="U51" t="s">
+      <c r="V51" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:22">
       <c r="A52" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3" t="b">
-        <v>0</v>
-      </c>
+      <c r="E52" s="3"/>
       <c r="F52" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="M52" s="3"/>
+      <c r="L52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-      <c r="U52" t="s">
+      <c r="S52" s="3"/>
+      <c r="V52" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:22">
       <c r="A53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3" t="b">
-        <v>1</v>
-      </c>
+      <c r="E53" s="3"/>
       <c r="F53" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G53" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="G53" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
-      <c r="L53" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="N53" s="3"/>
-      <c r="P53" s="3"/>
+      <c r="O53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
-      <c r="T53" t="s">
+      <c r="T53" s="3"/>
+      <c r="U53" t="s">
         <v>209</v>
       </c>
-      <c r="U53" t="s">
+      <c r="V53" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="54" spans="1:21">
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>59</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>264</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>65</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>157</v>
       </c>
-      <c r="F54" t="b">
-        <v>0</v>
-      </c>
-      <c r="T54" t="s">
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="U54" t="s">
         <v>210</v>
       </c>
-      <c r="U54" t="s">
+      <c r="V54" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>155</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>264</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>66</v>
       </c>
-      <c r="E55" t="b">
-        <v>0</v>
-      </c>
       <c r="F55" t="b">
-        <v>1</v>
-      </c>
-      <c r="T55" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="U55" t="s">
         <v>211</v>
       </c>
-      <c r="U55" t="s">
+      <c r="V55" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="1:21">
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>158</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>264</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>67</v>
       </c>
-      <c r="E56" t="b">
-        <v>0</v>
-      </c>
       <c r="F56" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="P56" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="S56" t="s">
+      <c r="T56" t="s">
         <v>160</v>
       </c>
-      <c r="T56" t="s">
+      <c r="U56" t="s">
         <v>212</v>
       </c>
-      <c r="U56" t="s">
+      <c r="V56" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3048,10 +3123,118 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7532,6 +7715,7 @@
     <hyperlink ref="W38" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7540,7 +7724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
test: update expressions in test files
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_datatypes.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_datatypes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/molgenis-platform-integration-tests/src/test/resources/xls/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461E961A-11B8-3E47-AEB4-8145D61D8DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22700" windowHeight="14720" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22700" windowHeight="14720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="5" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="it_emx_datatypes_TypeTest" sheetId="1" r:id="rId5"/>
     <sheet name="it_emx_datatypes_TypeTestRef" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -503,12 +509,6 @@
     <t>driverslicence</t>
   </si>
   <si>
-    <t>$('age').ge(18).value()</t>
-  </si>
-  <si>
-    <t>$('driverslicence').isNull().not().or($('age').isNull()).or($('age').lt(18)).value()</t>
-  </si>
-  <si>
     <t>defaultValue</t>
   </si>
   <si>
@@ -885,12 +885,18 @@
   </si>
   <si>
     <t>tags</t>
+  </si>
+  <si>
+    <t>{age}&gt;=18</t>
+  </si>
+  <si>
+    <t>driverslicence} notempty || {age} empty || {age} &lt; 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1056,6 +1062,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1347,20 +1356,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1371,28 +1380,28 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1407,14 +1416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1423,7 +1432,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1440,66 +1449,66 @@
         <v>140</v>
       </c>
       <c r="F1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
         <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>141</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
         <v>141</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>156</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
         <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1514,14 +1523,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="T56" sqref="T56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
@@ -1532,18 +1541,18 @@
     <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -1564,7 +1573,7 @@
         <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J1" t="s">
         <v>81</v>
@@ -1582,7 +1591,7 @@
         <v>91</v>
       </c>
       <c r="O1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P1" t="s">
         <v>92</v>
@@ -1606,15 +1615,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D2" t="s">
         <v>65</v>
@@ -1629,18 +1638,18 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="V2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
@@ -1658,21 +1667,21 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="V3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
         <v>66</v>
@@ -1687,15 +1696,15 @@
         <v>1</v>
       </c>
       <c r="V4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D5" t="s">
         <v>67</v>
@@ -1713,15 +1722,15 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
         <v>67</v>
@@ -1739,18 +1748,18 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="V6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
         <v>146</v>
@@ -1762,18 +1771,18 @@
         <v>0</v>
       </c>
       <c r="U7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D8" t="s">
         <v>66</v>
@@ -1794,15 +1803,15 @@
         <v>145</v>
       </c>
       <c r="V8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
         <v>65</v>
@@ -1823,24 +1832,24 @@
         <v>145</v>
       </c>
       <c r="U9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="V9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D10" t="s">
         <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1852,24 +1861,24 @@
         <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="V10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D11" t="s">
         <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -1881,21 +1890,21 @@
         <v>3</v>
       </c>
       <c r="U11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D12" t="s">
         <v>151</v>
       </c>
       <c r="E12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -1904,27 +1913,27 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O12" t="b">
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D13" t="s">
         <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -1933,18 +1942,18 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>
@@ -1962,18 +1971,18 @@
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
@@ -1988,18 +1997,18 @@
         <v>42095</v>
       </c>
       <c r="U15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="V15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -2014,15 +2023,15 @@
         <v>6</v>
       </c>
       <c r="V16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
@@ -2040,18 +2049,18 @@
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D18" t="s">
         <v>71</v>
@@ -2069,18 +2078,18 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="V18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -2095,18 +2104,18 @@
         <v>15.666</v>
       </c>
       <c r="U19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="V19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -2118,24 +2127,24 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O20" t="b">
         <v>1</v>
       </c>
       <c r="U20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="V20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
@@ -2150,18 +2159,18 @@
         <v>7</v>
       </c>
       <c r="U21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="V21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D22" t="s">
         <v>79</v>
@@ -2182,15 +2191,15 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D23" t="s">
         <v>79</v>
@@ -2208,18 +2217,18 @@
         <v>10</v>
       </c>
       <c r="U23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="V23" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D24" t="s">
         <v>73</v>
@@ -2234,15 +2243,15 @@
         <v>11</v>
       </c>
       <c r="V24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D25" t="s">
         <v>73</v>
@@ -2254,24 +2263,24 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="O25" t="b">
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="V25" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D26" t="s">
         <v>74</v>
@@ -2283,24 +2292,24 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="O26" t="b">
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="V26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D27" t="s">
         <v>74</v>
@@ -2312,21 +2321,21 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="V27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D28" t="s">
         <v>66</v>
@@ -2344,18 +2353,18 @@
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="V28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D29" t="s">
         <v>66</v>
@@ -2370,15 +2379,15 @@
         <v>1</v>
       </c>
       <c r="V29" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D30" t="s">
         <v>66</v>
@@ -2396,18 +2405,18 @@
         <v>10</v>
       </c>
       <c r="U30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="V30" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
@@ -2425,18 +2434,18 @@
         <v>0</v>
       </c>
       <c r="U31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="V31" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D32" t="s">
         <v>75</v>
@@ -2451,18 +2460,18 @@
         <v>12342151234</v>
       </c>
       <c r="U32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="V32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D33" t="s">
         <v>75</v>
@@ -2477,15 +2486,15 @@
         <v>12342151234</v>
       </c>
       <c r="V33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D34" t="s">
         <v>75</v>
@@ -2509,18 +2518,18 @@
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="V34" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D35" t="s">
         <v>75</v>
@@ -2544,24 +2553,24 @@
         <v>1</v>
       </c>
       <c r="U35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="V35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D36" t="s">
         <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2573,21 +2582,21 @@
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D37" t="s">
         <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2596,15 +2605,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D38" t="s">
         <v>65</v>
@@ -2622,18 +2631,18 @@
         <v>1</v>
       </c>
       <c r="U38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="V38" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D39" t="s">
         <v>65</v>
@@ -2648,18 +2657,18 @@
         <v>39</v>
       </c>
       <c r="U39" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="V39" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D40" t="s">
         <v>0</v>
@@ -2674,15 +2683,15 @@
         <v>40</v>
       </c>
       <c r="V40" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D41" t="s">
         <v>0</v>
@@ -2697,24 +2706,24 @@
         <v>41</v>
       </c>
       <c r="U41" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="V41" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D42" t="s">
         <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -2726,21 +2735,21 @@
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D43" t="s">
         <v>77</v>
       </c>
       <c r="E43" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -2749,15 +2758,15 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D44" t="s">
         <v>65</v>
@@ -2775,18 +2784,18 @@
         <v>0</v>
       </c>
       <c r="U44" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="V44" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D45" t="s">
         <v>65</v>
@@ -2798,24 +2807,24 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P45" t="b">
         <v>0</v>
       </c>
       <c r="U45" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="V45" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D46" t="s">
         <v>65</v>
@@ -2830,15 +2839,15 @@
         <v>1</v>
       </c>
       <c r="V46" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D47" t="s">
         <v>66</v>
@@ -2853,24 +2862,24 @@
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="V47" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>134</v>
       </c>
       <c r="C48" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D48" t="s">
         <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -2882,18 +2891,18 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D49" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -2902,18 +2911,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>139</v>
       </c>
       <c r="C50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D50" t="s">
         <v>77</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -2928,18 +2937,18 @@
         <v>142</v>
       </c>
       <c r="U50" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="V50" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D51" t="s">
         <v>66</v>
@@ -2957,19 +2966,19 @@
         <v>29</v>
       </c>
       <c r="U51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="V51" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>65</v>
@@ -2993,16 +3002,16 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="V52" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>66</v>
@@ -3029,18 +3038,18 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
       <c r="U53" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="V53" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D54" t="s">
         <v>65</v>
@@ -3052,18 +3061,18 @@
         <v>0</v>
       </c>
       <c r="U54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="V54" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D55" t="s">
         <v>66</v>
@@ -3075,18 +3084,18 @@
         <v>1</v>
       </c>
       <c r="U55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V55" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>158</v>
       </c>
       <c r="C56" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D56" t="s">
         <v>67</v>
@@ -3098,16 +3107,16 @@
         <v>1</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>159</v>
+        <v>285</v>
       </c>
       <c r="T56" t="s">
-        <v>160</v>
+        <v>286</v>
       </c>
       <c r="U56" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="V56" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3122,14 +3131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
@@ -3138,84 +3147,84 @@
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C1" t="s">
         <v>84</v>
       </c>
       <c r="D1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" t="s">
         <v>273</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>274</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" t="s">
         <v>276</v>
       </c>
-      <c r="B2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" t="s">
         <v>276</v>
       </c>
-      <c r="D2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" t="s">
         <v>277</v>
-      </c>
-      <c r="F2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" t="s">
-        <v>278</v>
-      </c>
-      <c r="E3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F4" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -3230,14 +3239,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AS39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -3267,7 +3276,7 @@
     <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -3401,10 +3410,10 @@
         <v>134</v>
       </c>
       <c r="AS1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3538,7 +3547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3752,7 +3761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3886,7 +3895,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4020,7 +4029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4097,7 +4106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4228,7 +4237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4359,7 +4368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4436,7 +4445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4567,7 +4576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:45">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4698,7 +4707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:45">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4775,7 +4784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:45">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:45">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5037,7 +5046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:45">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5114,7 +5123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5191,7 +5200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5322,7 +5331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5453,7 +5462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5530,7 +5539,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5661,7 +5670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:43">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5789,7 +5798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:43">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5863,7 +5872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:43">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5991,7 +6000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:43">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6119,7 +6128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:43">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6193,7 +6202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:43">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6321,7 +6330,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:43">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6449,7 +6458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:43">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6523,7 +6532,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:43">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6651,7 +6660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:43">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6779,7 +6788,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:43">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6853,7 +6862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:43">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6981,7 +6990,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:43">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -7109,7 +7118,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:43">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -7183,7 +7192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:43">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7257,7 +7266,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:43">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7385,7 +7394,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:43">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7513,7 +7522,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:43">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7589,130 +7598,130 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1"/>
-    <hyperlink ref="P3" r:id="rId2"/>
-    <hyperlink ref="Q2" r:id="rId3"/>
-    <hyperlink ref="P4" r:id="rId4"/>
-    <hyperlink ref="Q3" r:id="rId5"/>
-    <hyperlink ref="V2" r:id="rId6"/>
-    <hyperlink ref="V3" r:id="rId7"/>
-    <hyperlink ref="V4" r:id="rId8"/>
-    <hyperlink ref="W2" r:id="rId9"/>
-    <hyperlink ref="W3" r:id="rId10"/>
-    <hyperlink ref="P5" r:id="rId11"/>
-    <hyperlink ref="P6" r:id="rId12"/>
-    <hyperlink ref="Q5" r:id="rId13"/>
-    <hyperlink ref="P7" r:id="rId14"/>
-    <hyperlink ref="Q6" r:id="rId15"/>
-    <hyperlink ref="V5" r:id="rId16"/>
-    <hyperlink ref="V6" r:id="rId17"/>
-    <hyperlink ref="V7" r:id="rId18"/>
-    <hyperlink ref="W5" r:id="rId19"/>
-    <hyperlink ref="W6" r:id="rId20"/>
-    <hyperlink ref="P8" r:id="rId21"/>
-    <hyperlink ref="P9" r:id="rId22"/>
-    <hyperlink ref="Q8" r:id="rId23"/>
-    <hyperlink ref="P10" r:id="rId24"/>
-    <hyperlink ref="Q9" r:id="rId25"/>
-    <hyperlink ref="V8" r:id="rId26"/>
-    <hyperlink ref="V9" r:id="rId27"/>
-    <hyperlink ref="V10" r:id="rId28"/>
-    <hyperlink ref="W8" r:id="rId29"/>
-    <hyperlink ref="W9" r:id="rId30"/>
-    <hyperlink ref="P11" r:id="rId31"/>
-    <hyperlink ref="P12" r:id="rId32"/>
-    <hyperlink ref="Q11" r:id="rId33"/>
-    <hyperlink ref="P13" r:id="rId34"/>
-    <hyperlink ref="Q12" r:id="rId35"/>
-    <hyperlink ref="V11" r:id="rId36"/>
-    <hyperlink ref="V12" r:id="rId37"/>
-    <hyperlink ref="V13" r:id="rId38"/>
-    <hyperlink ref="W11" r:id="rId39"/>
-    <hyperlink ref="W12" r:id="rId40"/>
-    <hyperlink ref="P14" r:id="rId41"/>
-    <hyperlink ref="P15" r:id="rId42"/>
-    <hyperlink ref="Q14" r:id="rId43"/>
-    <hyperlink ref="P16" r:id="rId44"/>
-    <hyperlink ref="Q15" r:id="rId45"/>
-    <hyperlink ref="V14" r:id="rId46"/>
-    <hyperlink ref="V15" r:id="rId47"/>
-    <hyperlink ref="V16" r:id="rId48"/>
-    <hyperlink ref="W14" r:id="rId49"/>
-    <hyperlink ref="W15" r:id="rId50"/>
-    <hyperlink ref="P17" r:id="rId51"/>
-    <hyperlink ref="V17" r:id="rId52"/>
-    <hyperlink ref="P18" r:id="rId53"/>
-    <hyperlink ref="P19" r:id="rId54"/>
-    <hyperlink ref="Q18" r:id="rId55"/>
-    <hyperlink ref="P20" r:id="rId56"/>
-    <hyperlink ref="Q19" r:id="rId57"/>
-    <hyperlink ref="V18" r:id="rId58"/>
-    <hyperlink ref="V19" r:id="rId59"/>
-    <hyperlink ref="V20" r:id="rId60"/>
-    <hyperlink ref="W18" r:id="rId61"/>
-    <hyperlink ref="W19" r:id="rId62"/>
-    <hyperlink ref="P21" r:id="rId63"/>
-    <hyperlink ref="P22" r:id="rId64"/>
-    <hyperlink ref="Q21" r:id="rId65"/>
-    <hyperlink ref="P23" r:id="rId66"/>
-    <hyperlink ref="Q22" r:id="rId67"/>
-    <hyperlink ref="V21" r:id="rId68"/>
-    <hyperlink ref="V22" r:id="rId69"/>
-    <hyperlink ref="V23" r:id="rId70"/>
-    <hyperlink ref="W21" r:id="rId71"/>
-    <hyperlink ref="W22" r:id="rId72"/>
-    <hyperlink ref="P24" r:id="rId73"/>
-    <hyperlink ref="P25" r:id="rId74"/>
-    <hyperlink ref="Q24" r:id="rId75"/>
-    <hyperlink ref="P26" r:id="rId76"/>
-    <hyperlink ref="Q25" r:id="rId77"/>
-    <hyperlink ref="V24" r:id="rId78"/>
-    <hyperlink ref="V25" r:id="rId79"/>
-    <hyperlink ref="V26" r:id="rId80"/>
-    <hyperlink ref="W24" r:id="rId81"/>
-    <hyperlink ref="W25" r:id="rId82"/>
-    <hyperlink ref="P27" r:id="rId83"/>
-    <hyperlink ref="P28" r:id="rId84"/>
-    <hyperlink ref="Q27" r:id="rId85"/>
-    <hyperlink ref="P29" r:id="rId86"/>
-    <hyperlink ref="Q28" r:id="rId87"/>
-    <hyperlink ref="V27" r:id="rId88"/>
-    <hyperlink ref="V28" r:id="rId89"/>
-    <hyperlink ref="V29" r:id="rId90"/>
-    <hyperlink ref="W27" r:id="rId91"/>
-    <hyperlink ref="W28" r:id="rId92"/>
-    <hyperlink ref="P30" r:id="rId93"/>
-    <hyperlink ref="P31" r:id="rId94"/>
-    <hyperlink ref="Q30" r:id="rId95"/>
-    <hyperlink ref="P32" r:id="rId96"/>
-    <hyperlink ref="Q31" r:id="rId97"/>
-    <hyperlink ref="V30" r:id="rId98"/>
-    <hyperlink ref="V31" r:id="rId99"/>
-    <hyperlink ref="V32" r:id="rId100"/>
-    <hyperlink ref="W30" r:id="rId101"/>
-    <hyperlink ref="W31" r:id="rId102"/>
-    <hyperlink ref="P33" r:id="rId103"/>
-    <hyperlink ref="P34" r:id="rId104"/>
-    <hyperlink ref="Q33" r:id="rId105"/>
-    <hyperlink ref="P35" r:id="rId106"/>
-    <hyperlink ref="Q34" r:id="rId107"/>
-    <hyperlink ref="V33" r:id="rId108"/>
-    <hyperlink ref="V34" r:id="rId109"/>
-    <hyperlink ref="V35" r:id="rId110"/>
-    <hyperlink ref="W33" r:id="rId111"/>
-    <hyperlink ref="W34" r:id="rId112"/>
-    <hyperlink ref="P36" r:id="rId113"/>
-    <hyperlink ref="V36" r:id="rId114"/>
-    <hyperlink ref="P37" r:id="rId115"/>
-    <hyperlink ref="P38" r:id="rId116"/>
-    <hyperlink ref="Q37" r:id="rId117"/>
-    <hyperlink ref="P39" r:id="rId118"/>
-    <hyperlink ref="Q38" r:id="rId119"/>
-    <hyperlink ref="V37" r:id="rId120"/>
-    <hyperlink ref="V38" r:id="rId121"/>
-    <hyperlink ref="V39" r:id="rId122"/>
-    <hyperlink ref="W37" r:id="rId123"/>
-    <hyperlink ref="W38" r:id="rId124"/>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="Q2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="Q3" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="V2" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="V3" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="V4" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="W2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="W3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="P5" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="P6" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="Q5" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="P7" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="Q6" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="V5" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="V6" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="V7" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="W5" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="W6" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="P8" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="P9" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="Q8" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="P10" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="Q9" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="V8" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="V9" r:id="rId27" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="V10" r:id="rId28" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="W8" r:id="rId29" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="W9" r:id="rId30" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="P11" r:id="rId31" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="P12" r:id="rId32" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="Q11" r:id="rId33" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="P13" r:id="rId34" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="Q12" r:id="rId35" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="V11" r:id="rId36" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="V12" r:id="rId37" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="V13" r:id="rId38" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
+    <hyperlink ref="W11" r:id="rId39" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
+    <hyperlink ref="W12" r:id="rId40" xr:uid="{00000000-0004-0000-0400-000027000000}"/>
+    <hyperlink ref="P14" r:id="rId41" xr:uid="{00000000-0004-0000-0400-000028000000}"/>
+    <hyperlink ref="P15" r:id="rId42" xr:uid="{00000000-0004-0000-0400-000029000000}"/>
+    <hyperlink ref="Q14" r:id="rId43" xr:uid="{00000000-0004-0000-0400-00002A000000}"/>
+    <hyperlink ref="P16" r:id="rId44" xr:uid="{00000000-0004-0000-0400-00002B000000}"/>
+    <hyperlink ref="Q15" r:id="rId45" xr:uid="{00000000-0004-0000-0400-00002C000000}"/>
+    <hyperlink ref="V14" r:id="rId46" xr:uid="{00000000-0004-0000-0400-00002D000000}"/>
+    <hyperlink ref="V15" r:id="rId47" xr:uid="{00000000-0004-0000-0400-00002E000000}"/>
+    <hyperlink ref="V16" r:id="rId48" xr:uid="{00000000-0004-0000-0400-00002F000000}"/>
+    <hyperlink ref="W14" r:id="rId49" xr:uid="{00000000-0004-0000-0400-000030000000}"/>
+    <hyperlink ref="W15" r:id="rId50" xr:uid="{00000000-0004-0000-0400-000031000000}"/>
+    <hyperlink ref="P17" r:id="rId51" xr:uid="{00000000-0004-0000-0400-000032000000}"/>
+    <hyperlink ref="V17" r:id="rId52" xr:uid="{00000000-0004-0000-0400-000033000000}"/>
+    <hyperlink ref="P18" r:id="rId53" xr:uid="{00000000-0004-0000-0400-000034000000}"/>
+    <hyperlink ref="P19" r:id="rId54" xr:uid="{00000000-0004-0000-0400-000035000000}"/>
+    <hyperlink ref="Q18" r:id="rId55" xr:uid="{00000000-0004-0000-0400-000036000000}"/>
+    <hyperlink ref="P20" r:id="rId56" xr:uid="{00000000-0004-0000-0400-000037000000}"/>
+    <hyperlink ref="Q19" r:id="rId57" xr:uid="{00000000-0004-0000-0400-000038000000}"/>
+    <hyperlink ref="V18" r:id="rId58" xr:uid="{00000000-0004-0000-0400-000039000000}"/>
+    <hyperlink ref="V19" r:id="rId59" xr:uid="{00000000-0004-0000-0400-00003A000000}"/>
+    <hyperlink ref="V20" r:id="rId60" xr:uid="{00000000-0004-0000-0400-00003B000000}"/>
+    <hyperlink ref="W18" r:id="rId61" xr:uid="{00000000-0004-0000-0400-00003C000000}"/>
+    <hyperlink ref="W19" r:id="rId62" xr:uid="{00000000-0004-0000-0400-00003D000000}"/>
+    <hyperlink ref="P21" r:id="rId63" xr:uid="{00000000-0004-0000-0400-00003E000000}"/>
+    <hyperlink ref="P22" r:id="rId64" xr:uid="{00000000-0004-0000-0400-00003F000000}"/>
+    <hyperlink ref="Q21" r:id="rId65" xr:uid="{00000000-0004-0000-0400-000040000000}"/>
+    <hyperlink ref="P23" r:id="rId66" xr:uid="{00000000-0004-0000-0400-000041000000}"/>
+    <hyperlink ref="Q22" r:id="rId67" xr:uid="{00000000-0004-0000-0400-000042000000}"/>
+    <hyperlink ref="V21" r:id="rId68" xr:uid="{00000000-0004-0000-0400-000043000000}"/>
+    <hyperlink ref="V22" r:id="rId69" xr:uid="{00000000-0004-0000-0400-000044000000}"/>
+    <hyperlink ref="V23" r:id="rId70" xr:uid="{00000000-0004-0000-0400-000045000000}"/>
+    <hyperlink ref="W21" r:id="rId71" xr:uid="{00000000-0004-0000-0400-000046000000}"/>
+    <hyperlink ref="W22" r:id="rId72" xr:uid="{00000000-0004-0000-0400-000047000000}"/>
+    <hyperlink ref="P24" r:id="rId73" xr:uid="{00000000-0004-0000-0400-000048000000}"/>
+    <hyperlink ref="P25" r:id="rId74" xr:uid="{00000000-0004-0000-0400-000049000000}"/>
+    <hyperlink ref="Q24" r:id="rId75" xr:uid="{00000000-0004-0000-0400-00004A000000}"/>
+    <hyperlink ref="P26" r:id="rId76" xr:uid="{00000000-0004-0000-0400-00004B000000}"/>
+    <hyperlink ref="Q25" r:id="rId77" xr:uid="{00000000-0004-0000-0400-00004C000000}"/>
+    <hyperlink ref="V24" r:id="rId78" xr:uid="{00000000-0004-0000-0400-00004D000000}"/>
+    <hyperlink ref="V25" r:id="rId79" xr:uid="{00000000-0004-0000-0400-00004E000000}"/>
+    <hyperlink ref="V26" r:id="rId80" xr:uid="{00000000-0004-0000-0400-00004F000000}"/>
+    <hyperlink ref="W24" r:id="rId81" xr:uid="{00000000-0004-0000-0400-000050000000}"/>
+    <hyperlink ref="W25" r:id="rId82" xr:uid="{00000000-0004-0000-0400-000051000000}"/>
+    <hyperlink ref="P27" r:id="rId83" xr:uid="{00000000-0004-0000-0400-000052000000}"/>
+    <hyperlink ref="P28" r:id="rId84" xr:uid="{00000000-0004-0000-0400-000053000000}"/>
+    <hyperlink ref="Q27" r:id="rId85" xr:uid="{00000000-0004-0000-0400-000054000000}"/>
+    <hyperlink ref="P29" r:id="rId86" xr:uid="{00000000-0004-0000-0400-000055000000}"/>
+    <hyperlink ref="Q28" r:id="rId87" xr:uid="{00000000-0004-0000-0400-000056000000}"/>
+    <hyperlink ref="V27" r:id="rId88" xr:uid="{00000000-0004-0000-0400-000057000000}"/>
+    <hyperlink ref="V28" r:id="rId89" xr:uid="{00000000-0004-0000-0400-000058000000}"/>
+    <hyperlink ref="V29" r:id="rId90" xr:uid="{00000000-0004-0000-0400-000059000000}"/>
+    <hyperlink ref="W27" r:id="rId91" xr:uid="{00000000-0004-0000-0400-00005A000000}"/>
+    <hyperlink ref="W28" r:id="rId92" xr:uid="{00000000-0004-0000-0400-00005B000000}"/>
+    <hyperlink ref="P30" r:id="rId93" xr:uid="{00000000-0004-0000-0400-00005C000000}"/>
+    <hyperlink ref="P31" r:id="rId94" xr:uid="{00000000-0004-0000-0400-00005D000000}"/>
+    <hyperlink ref="Q30" r:id="rId95" xr:uid="{00000000-0004-0000-0400-00005E000000}"/>
+    <hyperlink ref="P32" r:id="rId96" xr:uid="{00000000-0004-0000-0400-00005F000000}"/>
+    <hyperlink ref="Q31" r:id="rId97" xr:uid="{00000000-0004-0000-0400-000060000000}"/>
+    <hyperlink ref="V30" r:id="rId98" xr:uid="{00000000-0004-0000-0400-000061000000}"/>
+    <hyperlink ref="V31" r:id="rId99" xr:uid="{00000000-0004-0000-0400-000062000000}"/>
+    <hyperlink ref="V32" r:id="rId100" xr:uid="{00000000-0004-0000-0400-000063000000}"/>
+    <hyperlink ref="W30" r:id="rId101" xr:uid="{00000000-0004-0000-0400-000064000000}"/>
+    <hyperlink ref="W31" r:id="rId102" xr:uid="{00000000-0004-0000-0400-000065000000}"/>
+    <hyperlink ref="P33" r:id="rId103" xr:uid="{00000000-0004-0000-0400-000066000000}"/>
+    <hyperlink ref="P34" r:id="rId104" xr:uid="{00000000-0004-0000-0400-000067000000}"/>
+    <hyperlink ref="Q33" r:id="rId105" xr:uid="{00000000-0004-0000-0400-000068000000}"/>
+    <hyperlink ref="P35" r:id="rId106" xr:uid="{00000000-0004-0000-0400-000069000000}"/>
+    <hyperlink ref="Q34" r:id="rId107" xr:uid="{00000000-0004-0000-0400-00006A000000}"/>
+    <hyperlink ref="V33" r:id="rId108" xr:uid="{00000000-0004-0000-0400-00006B000000}"/>
+    <hyperlink ref="V34" r:id="rId109" xr:uid="{00000000-0004-0000-0400-00006C000000}"/>
+    <hyperlink ref="V35" r:id="rId110" xr:uid="{00000000-0004-0000-0400-00006D000000}"/>
+    <hyperlink ref="W33" r:id="rId111" xr:uid="{00000000-0004-0000-0400-00006E000000}"/>
+    <hyperlink ref="W34" r:id="rId112" xr:uid="{00000000-0004-0000-0400-00006F000000}"/>
+    <hyperlink ref="P36" r:id="rId113" xr:uid="{00000000-0004-0000-0400-000070000000}"/>
+    <hyperlink ref="V36" r:id="rId114" xr:uid="{00000000-0004-0000-0400-000071000000}"/>
+    <hyperlink ref="P37" r:id="rId115" xr:uid="{00000000-0004-0000-0400-000072000000}"/>
+    <hyperlink ref="P38" r:id="rId116" xr:uid="{00000000-0004-0000-0400-000073000000}"/>
+    <hyperlink ref="Q37" r:id="rId117" xr:uid="{00000000-0004-0000-0400-000074000000}"/>
+    <hyperlink ref="P39" r:id="rId118" xr:uid="{00000000-0004-0000-0400-000075000000}"/>
+    <hyperlink ref="Q38" r:id="rId119" xr:uid="{00000000-0004-0000-0400-000076000000}"/>
+    <hyperlink ref="V37" r:id="rId120" xr:uid="{00000000-0004-0000-0400-000077000000}"/>
+    <hyperlink ref="V38" r:id="rId121" xr:uid="{00000000-0004-0000-0400-000078000000}"/>
+    <hyperlink ref="V39" r:id="rId122" xr:uid="{00000000-0004-0000-0400-000079000000}"/>
+    <hyperlink ref="W37" r:id="rId123" xr:uid="{00000000-0004-0000-0400-00007A000000}"/>
+    <hyperlink ref="W38" r:id="rId124" xr:uid="{00000000-0004-0000-0400-00007B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7725,16 +7734,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7742,7 +7751,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7750,7 +7759,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -7758,7 +7767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -7766,7 +7775,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -7774,7 +7783,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>

</xml_diff>